<commit_message>
Updated README including environment setup for large messages
</commit_message>
<xml_diff>
--- a/results/Kafka_Results.xlsx
+++ b/results/Kafka_Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JNEATE\Documents\IKEA\Kafka\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\Event-Hub-PoC\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11024EB2-A762-4BC2-A7EF-3BCA7B1D79D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776E138D-A4C0-4B02-8F44-806AF92314C8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="456" windowWidth="28284" windowHeight="17076" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
   <si>
     <t>Concurrent Threads</t>
   </si>
@@ -88,7 +88,7 @@
     <t>PEND</t>
   </si>
   <si>
-    <t>WIP</t>
+    <t>103m 7s</t>
   </si>
 </sst>
 </file>
@@ -97,8 +97,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -116,18 +116,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,18 +137,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -444,7 +437,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -509,11 +502,11 @@
         <v>10.9</v>
       </c>
       <c r="E2">
-        <f>B2*C2</f>
+        <f t="shared" ref="E2:E9" si="0">B2*C2</f>
         <v>1000</v>
       </c>
       <c r="F2" s="4">
-        <f>(D2*E2)/1024</f>
+        <f t="shared" ref="F2:F9" si="1">(D2*E2)/1024</f>
         <v>10.64453125</v>
       </c>
       <c r="G2" t="s">
@@ -547,11 +540,11 @@
         <v>10.9</v>
       </c>
       <c r="E3" s="2">
-        <f>B3*C3</f>
+        <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="F3" s="4">
-        <f>(D3*E3)/1024</f>
+        <f t="shared" si="1"/>
         <v>1064.453125</v>
       </c>
       <c r="G3" t="s">
@@ -572,7 +565,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A6" si="0">A3+1</f>
+        <f t="shared" ref="A4:A6" si="2">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4">
@@ -585,11 +578,11 @@
         <v>10.9</v>
       </c>
       <c r="E4" s="2">
-        <f>B4*C4</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="F4" s="4">
-        <f>(D4*E4)/1024</f>
+        <f t="shared" si="1"/>
         <v>106.4453125</v>
       </c>
       <c r="G4" t="s">
@@ -610,7 +603,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="B5">
@@ -623,50 +616,50 @@
         <v>10.9</v>
       </c>
       <c r="E5" s="2">
-        <f>B5*C5</f>
+        <f t="shared" si="0"/>
         <v>100000</v>
       </c>
       <c r="F5" s="4">
-        <f>(D5*E5)/1024</f>
+        <f t="shared" si="1"/>
         <v>1064.453125</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>19</v>
+      <c r="H5" s="1">
+        <v>812</v>
+      </c>
+      <c r="I5" s="1">
+        <v>891</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1551</v>
+      </c>
+      <c r="K5" s="1">
+        <v>3097</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>150</v>
+      </c>
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>100</v>
-      </c>
-      <c r="E6" s="2">
-        <f>B6*C6</f>
         <v>1</v>
       </c>
       <c r="F6" s="4">
-        <f>(D6*E6)/1024</f>
-        <v>9.765625E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.146484375</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>
@@ -695,15 +688,15 @@
         <v>10</v>
       </c>
       <c r="D7" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E7" s="2">
-        <f>B7*C7</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="F7" s="4">
-        <f>(D7*E7)/1024</f>
-        <v>0.9765625</v>
+        <f t="shared" si="1"/>
+        <v>1.46484375</v>
       </c>
       <c r="G7" t="s">
         <v>18</v>
@@ -732,15 +725,15 @@
         <v>100</v>
       </c>
       <c r="D8" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E8" s="2">
-        <f>B8*C8</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="F8" s="4">
-        <f>(D8*E8)/1024</f>
-        <v>97.65625</v>
+        <f t="shared" si="1"/>
+        <v>146.484375</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
@@ -769,15 +762,15 @@
         <v>1000</v>
       </c>
       <c r="D9" s="3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E9" s="2">
-        <f>B9*C9</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="F9" s="4">
-        <f>(D9*E9)/1024</f>
-        <v>976.5625</v>
+        <f t="shared" si="1"/>
+        <v>1464.84375</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
@@ -878,7 +871,7 @@
       <c r="C2" s="2">
         <v>10000</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <f>B2*C2</f>
         <v>10000</v>
       </c>
@@ -919,7 +912,7 @@
       <c r="C3" s="2">
         <v>10000</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <f>B3*C3</f>
         <v>10000</v>
       </c>
@@ -967,66 +960,66 @@
       <c r="L4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
+      <c r="A31" s="6"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
+      <c r="A32" s="6"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="6"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
+      <c r="A34" s="6"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
+      <c r="A35" s="6"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+      <c r="A36" s="6"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
+      <c r="A37" s="6"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
+      <c r="A38" s="6"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
+      <c r="A39" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>